<commit_message>
Finished CHC identification for Flying/Not Flying experiment, finishing group table creation.
</commit_message>
<xml_diff>
--- a/data/raw/Flying/tmp/Ib-FALSE_RT_ID_table.xlsx
+++ b/data/raw/Flying/tmp/Ib-FALSE_RT_ID_table.xlsx
@@ -19,8 +19,131 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B165" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">FUSE peaks
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B183" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 181, 182</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B184" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 183 &amp; 184</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B195" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 194 &amp; 195</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B222" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 221, 222, 223</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B231" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 230 &amp; 231</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B238" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 237 &amp; 238</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B256" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuse 255 &amp; 256</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="341">
   <si>
     <t xml:space="preserve">Peak</t>
   </si>
@@ -532,6 +655,9 @@
     <t xml:space="preserve">P148</t>
   </si>
   <si>
+    <t xml:space="preserve">C22_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P149</t>
   </si>
   <si>
@@ -544,6 +670,9 @@
     <t xml:space="preserve">P152</t>
   </si>
   <si>
+    <t xml:space="preserve">C22_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P153</t>
   </si>
   <si>
@@ -565,9 +694,15 @@
     <t xml:space="preserve">P159</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P160</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P161</t>
   </si>
   <si>
@@ -577,6 +712,9 @@
     <t xml:space="preserve">P163</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P164</t>
   </si>
   <si>
@@ -589,6 +727,9 @@
     <t xml:space="preserve">P167</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_Me_11-</t>
+  </si>
+  <si>
     <t xml:space="preserve">P168</t>
   </si>
   <si>
@@ -601,6 +742,9 @@
     <t xml:space="preserve">P171</t>
   </si>
   <si>
+    <t xml:space="preserve">C24_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P172</t>
   </si>
   <si>
@@ -610,6 +754,9 @@
     <t xml:space="preserve">P174</t>
   </si>
   <si>
+    <t xml:space="preserve">C24_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P175</t>
   </si>
   <si>
@@ -634,6 +781,9 @@
     <t xml:space="preserve">P182</t>
   </si>
   <si>
+    <t xml:space="preserve">C25_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P183</t>
   </si>
   <si>
@@ -646,6 +796,9 @@
     <t xml:space="preserve">P186</t>
   </si>
   <si>
+    <t xml:space="preserve">C25_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P187</t>
   </si>
   <si>
@@ -670,12 +823,18 @@
     <t xml:space="preserve">P194</t>
   </si>
   <si>
+    <t xml:space="preserve">C26_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P195</t>
   </si>
   <si>
     <t xml:space="preserve">P196</t>
   </si>
   <si>
+    <t xml:space="preserve">C26_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P197</t>
   </si>
   <si>
@@ -700,6 +859,9 @@
     <t xml:space="preserve">P204</t>
   </si>
   <si>
+    <t xml:space="preserve">C27_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P205</t>
   </si>
   <si>
@@ -709,12 +871,18 @@
     <t xml:space="preserve">P207</t>
   </si>
   <si>
+    <t xml:space="preserve">C27_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P208</t>
   </si>
   <si>
     <t xml:space="preserve">P209</t>
   </si>
   <si>
+    <t xml:space="preserve">C27_Me_11;13-</t>
+  </si>
+  <si>
     <t xml:space="preserve">P210</t>
   </si>
   <si>
@@ -730,6 +898,9 @@
     <t xml:space="preserve">P214</t>
   </si>
   <si>
+    <t xml:space="preserve">C28_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P215</t>
   </si>
   <si>
@@ -751,6 +922,9 @@
     <t xml:space="preserve">P221</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P222</t>
   </si>
   <si>
@@ -760,12 +934,18 @@
     <t xml:space="preserve">P224</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P225</t>
   </si>
   <si>
     <t xml:space="preserve">P226</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_Me_11;13-</t>
+  </si>
+  <si>
     <t xml:space="preserve">P227</t>
   </si>
   <si>
@@ -778,6 +958,9 @@
     <t xml:space="preserve">P230</t>
   </si>
   <si>
+    <t xml:space="preserve">C30_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P231</t>
   </si>
   <si>
@@ -787,6 +970,9 @@
     <t xml:space="preserve">P233</t>
   </si>
   <si>
+    <t xml:space="preserve">C30_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P234</t>
   </si>
   <si>
@@ -799,6 +985,9 @@
     <t xml:space="preserve">P237</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P238</t>
   </si>
   <si>
@@ -808,18 +997,27 @@
     <t xml:space="preserve">P240</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P241</t>
   </si>
   <si>
     <t xml:space="preserve">P242</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P243</t>
   </si>
   <si>
     <t xml:space="preserve">P244</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_Me_13;15-</t>
+  </si>
+  <si>
     <t xml:space="preserve">P245</t>
   </si>
   <si>
@@ -832,6 +1030,9 @@
     <t xml:space="preserve">P248</t>
   </si>
   <si>
+    <t xml:space="preserve">C32_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P249</t>
   </si>
   <si>
@@ -853,10 +1054,16 @@
     <t xml:space="preserve">P255</t>
   </si>
   <si>
+    <t xml:space="preserve">C33_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P256</t>
   </si>
   <si>
     <t xml:space="preserve">P257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33_ane_NA</t>
   </si>
   <si>
     <t xml:space="preserve">P258</t>
@@ -992,7 +1199,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,8 +1208,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFFFFFD7"/>
       </patternFill>
     </fill>
   </fills>
@@ -1040,12 +1253,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1058,6 +1279,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFD7"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFFA6"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1069,14 +1350,14 @@
   <dimension ref="A1:M292"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E151" activeCellId="0" sqref="E151"/>
+      <selection pane="bottomLeft" activeCell="B259" activeCellId="0" sqref="B259"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4532,6 +4813,9 @@
       <c r="A149" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="B149" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="C149" s="1" t="n">
         <v>30.698</v>
       </c>
@@ -4565,6 +4849,9 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B150" s="0" t="s">
         <v>170</v>
       </c>
       <c r="C150" s="0" t="n">
@@ -4603,7 +4890,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C151" s="0" t="n">
         <v>30.993</v>
@@ -4614,7 +4901,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C152" s="0" t="n">
         <v>31.0718</v>
@@ -4637,7 +4924,10 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>175</v>
       </c>
       <c r="C153" s="0" t="n">
         <v>31.1769</v>
@@ -4675,7 +4965,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C154" s="0" t="n">
         <v>31.395</v>
@@ -4692,7 +4982,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C155" s="0" t="n">
         <v>31.6069</v>
@@ -4730,7 +5020,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C156" s="0" t="n">
         <v>31.7376666666667</v>
@@ -4747,7 +5037,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C157" s="0" t="n">
         <v>31.9901</v>
@@ -4785,7 +5075,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C158" s="0" t="n">
         <v>32.089</v>
@@ -4796,7 +5086,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C159" s="0" t="n">
         <v>32.231</v>
@@ -4831,7 +5121,10 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>183</v>
       </c>
       <c r="C160" s="0" t="n">
         <v>32.3247</v>
@@ -4869,7 +5162,10 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>185</v>
       </c>
       <c r="C161" s="0" t="n">
         <v>32.4389</v>
@@ -4907,7 +5203,10 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>185</v>
       </c>
       <c r="C162" s="0" t="n">
         <v>32.5404</v>
@@ -4945,7 +5244,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C163" s="0" t="n">
         <v>32.6688888888889</v>
@@ -4980,7 +5279,10 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>189</v>
       </c>
       <c r="C164" s="0" t="n">
         <v>32.9766666666667</v>
@@ -5006,21 +5308,24 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>189</v>
       </c>
       <c r="C165" s="0" t="n">
         <v>33.0623</v>
       </c>
-      <c r="D165" s="0" t="n">
+      <c r="D165" s="2" t="n">
         <v>33.096</v>
       </c>
       <c r="E165" s="0" t="n">
         <v>33.061</v>
       </c>
-      <c r="F165" s="0" t="n">
+      <c r="F165" s="2" t="n">
         <v>33.068</v>
       </c>
-      <c r="G165" s="0" t="n">
+      <c r="G165" s="2" t="n">
         <v>33.069</v>
       </c>
       <c r="H165" s="0" t="n">
@@ -5035,7 +5340,7 @@
       <c r="K165" s="0" t="n">
         <v>33.068</v>
       </c>
-      <c r="L165" s="0" t="n">
+      <c r="L165" s="2" t="n">
         <v>33.027</v>
       </c>
       <c r="M165" s="0" t="n">
@@ -5044,7 +5349,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C166" s="0" t="n">
         <v>33.089</v>
@@ -5055,7 +5360,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C167" s="0" t="n">
         <v>33.3319</v>
@@ -5093,7 +5398,10 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>188</v>
+        <v>193</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>194</v>
       </c>
       <c r="C168" s="0" t="n">
         <v>33.4499</v>
@@ -5131,7 +5439,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C169" s="0" t="n">
         <v>33.56325</v>
@@ -5163,7 +5471,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C170" s="0" t="n">
         <v>33.668</v>
@@ -5174,7 +5482,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C171" s="0" t="n">
         <v>33.8701428571429</v>
@@ -5203,7 +5511,10 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>199</v>
       </c>
       <c r="C172" s="0" t="n">
         <v>34.0423</v>
@@ -5241,7 +5552,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C173" s="0" t="n">
         <v>34.1546</v>
@@ -5279,7 +5590,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C174" s="0" t="n">
         <v>34.427</v>
@@ -5290,7 +5601,10 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>195</v>
+        <v>202</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>203</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>34.4757</v>
@@ -5328,7 +5642,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C176" s="0" t="n">
         <v>34.6682</v>
@@ -5351,7 +5665,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C177" s="0" t="n">
         <v>34.79</v>
@@ -5368,7 +5682,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C178" s="0" t="n">
         <v>34.93</v>
@@ -5406,7 +5720,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C179" s="0" t="n">
         <v>35.0764</v>
@@ -5429,7 +5743,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C180" s="0" t="n">
         <v>35.2186</v>
@@ -5467,7 +5781,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C181" s="0" t="n">
         <v>35.39075</v>
@@ -5487,7 +5801,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C182" s="0" t="n">
         <v>35.55975</v>
@@ -5507,7 +5821,10 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>203</v>
+        <v>211</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>212</v>
       </c>
       <c r="C183" s="0" t="n">
         <v>35.6475</v>
@@ -5545,7 +5862,10 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>204</v>
+        <v>213</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>212</v>
       </c>
       <c r="C184" s="0" t="n">
         <v>35.726</v>
@@ -5577,7 +5897,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C185" s="0" t="n">
         <v>35.7671666666667</v>
@@ -5603,7 +5923,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C186" s="0" t="n">
         <v>35.8912222222222</v>
@@ -5638,7 +5958,10 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>207</v>
+        <v>216</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>217</v>
       </c>
       <c r="C187" s="0" t="n">
         <v>36.1793</v>
@@ -5676,7 +5999,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="C188" s="0" t="n">
         <v>36.2586666666667</v>
@@ -5702,7 +6025,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="C189" s="0" t="n">
         <v>36.3188</v>
@@ -5725,7 +6048,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="C190" s="0" t="n">
         <v>36.5258</v>
@@ -5763,7 +6086,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C191" s="0" t="n">
         <v>36.612</v>
@@ -5774,7 +6097,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="C192" s="0" t="n">
         <v>36.688</v>
@@ -5785,7 +6108,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C193" s="0" t="n">
         <v>36.7962</v>
@@ -5823,7 +6146,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="C194" s="0" t="n">
         <v>36.9711111111111</v>
@@ -5858,7 +6181,10 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>226</v>
       </c>
       <c r="C195" s="0" t="n">
         <v>37.13075</v>
@@ -5890,7 +6216,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="C196" s="0" t="n">
         <v>37.2286</v>
@@ -5928,7 +6254,10 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>217</v>
+        <v>228</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>229</v>
       </c>
       <c r="C197" s="0" t="n">
         <v>37.5222</v>
@@ -5966,7 +6295,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="C198" s="0" t="n">
         <v>37.7183333333333</v>
@@ -5983,7 +6312,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C199" s="0" t="n">
         <v>37.7955</v>
@@ -5997,7 +6326,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="C200" s="0" t="n">
         <v>37.885</v>
@@ -6017,7 +6346,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="C201" s="0" t="n">
         <v>37.9989</v>
@@ -6055,7 +6384,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="C202" s="0" t="n">
         <v>38.095</v>
@@ -6090,7 +6419,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="C203" s="0" t="n">
         <v>38.1766</v>
@@ -6128,7 +6457,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="C204" s="0" t="n">
         <v>38.3713333333333</v>
@@ -6145,7 +6474,10 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>225</v>
+        <v>237</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="C205" s="0" t="n">
         <v>38.6164</v>
@@ -6183,7 +6515,10 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>226</v>
+        <v>239</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="C206" s="0" t="n">
         <v>38.7228</v>
@@ -6221,7 +6556,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C207" s="0" t="n">
         <v>38.819</v>
@@ -6232,7 +6567,10 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>228</v>
+        <v>241</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>242</v>
       </c>
       <c r="C208" s="0" t="n">
         <v>39.1131</v>
@@ -6270,7 +6608,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="C209" s="0" t="n">
         <v>39.2379</v>
@@ -6308,7 +6646,10 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>230</v>
+        <v>244</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="C210" s="0" t="n">
         <v>39.4266</v>
@@ -6346,7 +6687,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="C211" s="0" t="n">
         <v>39.6564</v>
@@ -6384,7 +6725,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="C212" s="0" t="n">
         <v>39.808625</v>
@@ -6416,7 +6757,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="C213" s="0" t="n">
         <v>39.9975555555556</v>
@@ -6451,7 +6792,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="C214" s="0" t="n">
         <v>40.0936</v>
@@ -6489,7 +6830,10 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>235</v>
+        <v>250</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>251</v>
       </c>
       <c r="C215" s="0" t="n">
         <v>40.3451</v>
@@ -6527,7 +6871,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="C216" s="0" t="n">
         <v>40.6202</v>
@@ -6550,7 +6894,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="C217" s="0" t="n">
         <v>40.766</v>
@@ -6588,7 +6932,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C218" s="0" t="n">
         <v>40.8535</v>
@@ -6602,7 +6946,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="C219" s="0" t="n">
         <v>41.0036</v>
@@ -6640,7 +6984,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="C220" s="0" t="n">
         <v>41.1072</v>
@@ -6663,7 +7007,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C221" s="0" t="n">
         <v>41.205</v>
@@ -6680,7 +7024,10 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>242</v>
+        <v>258</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>259</v>
       </c>
       <c r="C222" s="0" t="n">
         <v>41.3898</v>
@@ -6718,7 +7065,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="C223" s="0" t="n">
         <v>41.448</v>
@@ -6738,7 +7085,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="C224" s="0" t="n">
         <v>41.4971666666667</v>
@@ -6764,7 +7111,10 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>245</v>
+        <v>262</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>263</v>
       </c>
       <c r="C225" s="0" t="n">
         <v>41.7636</v>
@@ -6802,7 +7152,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="C226" s="0" t="n">
         <v>41.961</v>
@@ -6840,7 +7190,10 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>247</v>
+        <v>265</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>266</v>
       </c>
       <c r="C227" s="0" t="n">
         <v>42.0974</v>
@@ -6878,7 +7231,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="C228" s="0" t="n">
         <v>42.219</v>
@@ -6889,7 +7242,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="C229" s="0" t="n">
         <v>42.3438571428571</v>
@@ -6918,7 +7271,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="C230" s="0" t="n">
         <v>42.4816</v>
@@ -6956,7 +7309,10 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>251</v>
+        <v>270</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>271</v>
       </c>
       <c r="C231" s="0" t="n">
         <v>42.7106666666667</v>
@@ -6991,7 +7347,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="C232" s="0" t="n">
         <v>42.798</v>
@@ -7008,7 +7364,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="C233" s="0" t="n">
         <v>42.8648</v>
@@ -7046,7 +7402,10 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>254</v>
+        <v>274</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>275</v>
       </c>
       <c r="C234" s="0" t="n">
         <v>42.9819</v>
@@ -7084,7 +7443,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="C235" s="0" t="n">
         <v>43.246</v>
@@ -7095,7 +7454,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="C236" s="0" t="n">
         <v>43.3545714285714</v>
@@ -7124,7 +7483,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="C237" s="0" t="n">
         <v>43.4628888888889</v>
@@ -7159,7 +7518,10 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>258</v>
+        <v>279</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>280</v>
       </c>
       <c r="C238" s="0" t="n">
         <v>43.649</v>
@@ -7188,7 +7550,10 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>259</v>
+        <v>281</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>280</v>
       </c>
       <c r="C239" s="0" t="n">
         <v>43.7345</v>
@@ -7226,7 +7591,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="C240" s="0" t="n">
         <v>43.8591111111111</v>
@@ -7261,7 +7626,10 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>261</v>
+        <v>283</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>284</v>
       </c>
       <c r="C241" s="0" t="n">
         <v>43.9476</v>
@@ -7299,7 +7667,10 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>262</v>
+        <v>285</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>284</v>
       </c>
       <c r="C242" s="0" t="n">
         <v>44.0396</v>
@@ -7337,7 +7708,10 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>263</v>
+        <v>286</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>287</v>
       </c>
       <c r="C243" s="0" t="n">
         <v>44.2715</v>
@@ -7375,7 +7749,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="C244" s="0" t="n">
         <v>44.529</v>
@@ -7386,7 +7760,10 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>265</v>
+        <v>289</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="C245" s="0" t="n">
         <v>44.6058</v>
@@ -7424,7 +7801,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="C246" s="0" t="n">
         <v>44.732</v>
@@ -7438,7 +7815,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="C247" s="0" t="n">
         <v>44.89</v>
@@ -7467,7 +7844,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="C248" s="0" t="n">
         <v>44.9405</v>
@@ -7487,7 +7864,10 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>269</v>
+        <v>294</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C249" s="0" t="n">
         <v>45.1874</v>
@@ -7525,7 +7905,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="C250" s="0" t="n">
         <v>45.344</v>
@@ -7545,7 +7925,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="C251" s="0" t="n">
         <v>45.4082</v>
@@ -7583,7 +7963,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>272</v>
+        <v>298</v>
       </c>
       <c r="C252" s="0" t="n">
         <v>45.473</v>
@@ -7594,7 +7974,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c r="C253" s="0" t="n">
         <v>45.6334444444444</v>
@@ -7629,7 +8009,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="C254" s="0" t="n">
         <v>45.839</v>
@@ -7652,7 +8032,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="C255" s="0" t="n">
         <v>46.119</v>
@@ -7690,7 +8070,10 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>276</v>
+        <v>302</v>
+      </c>
+      <c r="B256" s="0" t="s">
+        <v>303</v>
       </c>
       <c r="C256" s="0" t="n">
         <v>46.3796</v>
@@ -7728,7 +8111,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="C257" s="0" t="n">
         <v>46.46425</v>
@@ -7748,7 +8131,10 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>278</v>
+        <v>305</v>
+      </c>
+      <c r="B258" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="C258" s="0" t="n">
         <v>46.6396</v>
@@ -7786,7 +8172,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="C259" s="0" t="n">
         <v>46.795</v>
@@ -7824,7 +8210,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="C260" s="0" t="n">
         <v>47.0144</v>
@@ -7862,7 +8248,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>281</v>
+        <v>309</v>
       </c>
       <c r="C261" s="0" t="n">
         <v>47.1245</v>
@@ -7876,7 +8262,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>282</v>
+        <v>310</v>
       </c>
       <c r="C262" s="0" t="n">
         <v>47.25575</v>
@@ -7896,7 +8282,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>283</v>
+        <v>311</v>
       </c>
       <c r="C263" s="0" t="n">
         <v>47.3841</v>
@@ -7934,7 +8320,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>284</v>
+        <v>312</v>
       </c>
       <c r="C264" s="0" t="n">
         <v>47.487</v>
@@ -7945,7 +8331,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="C265" s="0" t="n">
         <v>47.6571428571429</v>
@@ -7974,7 +8360,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>286</v>
+        <v>314</v>
       </c>
       <c r="C266" s="0" t="n">
         <v>47.797</v>
@@ -8006,7 +8392,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>287</v>
+        <v>315</v>
       </c>
       <c r="C267" s="0" t="n">
         <v>47.907</v>
@@ -8017,7 +8403,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="C268" s="0" t="n">
         <v>48.214</v>
@@ -8031,7 +8417,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="C269" s="0" t="n">
         <v>48.364</v>
@@ -8069,7 +8455,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
       <c r="C270" s="0" t="n">
         <v>48.5601666666667</v>
@@ -8095,7 +8481,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>291</v>
+        <v>319</v>
       </c>
       <c r="C271" s="0" t="n">
         <v>48.676</v>
@@ -8109,7 +8495,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="C272" s="0" t="n">
         <v>48.866</v>
@@ -8147,7 +8533,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="C273" s="0" t="n">
         <v>49.052</v>
@@ -8158,7 +8544,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="C274" s="0" t="n">
         <v>49.2315</v>
@@ -8172,7 +8558,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>295</v>
+        <v>323</v>
       </c>
       <c r="C275" s="0" t="n">
         <v>49.369</v>
@@ -8183,7 +8569,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>296</v>
+        <v>324</v>
       </c>
       <c r="C276" s="0" t="n">
         <v>49.691</v>
@@ -8200,7 +8586,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="C277" s="0" t="n">
         <v>49.8891428571429</v>
@@ -8229,7 +8615,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="C278" s="0" t="n">
         <v>50.0256</v>
@@ -8252,7 +8638,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
       <c r="C279" s="0" t="n">
         <v>50.183</v>
@@ -8263,7 +8649,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="C280" s="0" t="n">
         <v>50.7</v>
@@ -8274,7 +8660,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="C281" s="0" t="n">
         <v>50.9116666666667</v>
@@ -8291,7 +8677,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="C282" s="0" t="n">
         <v>51.3585</v>
@@ -8305,7 +8691,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="C283" s="0" t="n">
         <v>51.658</v>
@@ -8316,7 +8702,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="C284" s="0" t="n">
         <v>52.161</v>
@@ -8348,7 +8734,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="C285" s="0" t="n">
         <v>52.486</v>
@@ -8371,7 +8757,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>306</v>
+        <v>334</v>
       </c>
       <c r="C286" s="0" t="n">
         <v>52.761</v>
@@ -8382,7 +8768,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
       <c r="C287" s="0" t="n">
         <v>53.6836666666667</v>
@@ -8399,7 +8785,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>308</v>
+        <v>336</v>
       </c>
       <c r="C288" s="0" t="n">
         <v>53.872</v>
@@ -8413,7 +8799,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>309</v>
+        <v>337</v>
       </c>
       <c r="C289" s="0" t="n">
         <v>54.9088</v>
@@ -8436,7 +8822,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="C290" s="0" t="n">
         <v>55.9081</v>
@@ -8474,7 +8860,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>311</v>
+        <v>339</v>
       </c>
       <c r="C291" s="0" t="n">
         <v>56.4405</v>
@@ -8488,7 +8874,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="C292" s="0" t="n">
         <v>57.5265</v>
@@ -8514,5 +8900,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>